<commit_message>
fixed issue with formatting of one row
</commit_message>
<xml_diff>
--- a/examples/Data/imdb.xlsx
+++ b/examples/Data/imdb.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessia/Documents/DataScience/textconsultations/examples/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A90665-BBCB-604D-9E3B-E1258414AD9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EB3866-1C6E-C043-8BEE-563344BD369E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15680" xr2:uid="{523911B3-8548-B847-84BC-0C598EE7205A}"/>
   </bookViews>
@@ -2486,12 +2486,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2808,10 +2805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35767422-A7CD-F748-BB92-C79ABDCD6175}">
-  <dimension ref="A1:B747"/>
+  <dimension ref="A1:B746"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A723" workbookViewId="0">
-      <selection activeCell="C476" sqref="C476"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A590" sqref="A590:XFD590"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7529,8 +7526,8 @@
       </c>
     </row>
     <row r="590" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A590" s="2">
-        <v>43383</v>
+      <c r="A590" s="1" t="s">
+        <v>587</v>
       </c>
       <c r="B590">
         <v>1</v>
@@ -7538,7 +7535,7 @@
     </row>
     <row r="591" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A591" s="1" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B591">
         <v>1</v>
@@ -7546,7 +7543,7 @@
     </row>
     <row r="592" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A592" s="1" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B592">
         <v>1</v>
@@ -7554,7 +7551,7 @@
     </row>
     <row r="593" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A593" s="1" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B593">
         <v>1</v>
@@ -7562,7 +7559,7 @@
     </row>
     <row r="594" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A594" s="1" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B594">
         <v>1</v>
@@ -7570,7 +7567,7 @@
     </row>
     <row r="595" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A595" s="1" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B595">
         <v>1</v>
@@ -7578,7 +7575,7 @@
     </row>
     <row r="596" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A596" s="1" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B596">
         <v>1</v>
@@ -7586,7 +7583,7 @@
     </row>
     <row r="597" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A597" s="1" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B597">
         <v>1</v>
@@ -7594,7 +7591,7 @@
     </row>
     <row r="598" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A598" s="1" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="B598">
         <v>1</v>
@@ -7602,7 +7599,7 @@
     </row>
     <row r="599" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A599" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B599">
         <v>1</v>
@@ -7610,15 +7607,15 @@
     </row>
     <row r="600" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A600" s="1" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B600">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="601" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A601" s="1" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B601">
         <v>0</v>
@@ -7626,7 +7623,7 @@
     </row>
     <row r="602" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A602" s="1" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B602">
         <v>0</v>
@@ -7634,7 +7631,7 @@
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A603" s="1" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B603">
         <v>0</v>
@@ -7642,7 +7639,7 @@
     </row>
     <row r="604" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A604" s="1" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B604">
         <v>0</v>
@@ -7650,7 +7647,7 @@
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A605" s="1" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="B605">
         <v>0</v>
@@ -7658,7 +7655,7 @@
     </row>
     <row r="606" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A606" s="1" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B606">
         <v>0</v>
@@ -7666,7 +7663,7 @@
     </row>
     <row r="607" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A607" s="1" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B607">
         <v>0</v>
@@ -7674,15 +7671,15 @@
     </row>
     <row r="608" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A608" s="1" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B608">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="609" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A609" s="1" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B609">
         <v>1</v>
@@ -7690,7 +7687,7 @@
     </row>
     <row r="610" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A610" s="1" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B610">
         <v>1</v>
@@ -7698,7 +7695,7 @@
     </row>
     <row r="611" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A611" s="1" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B611">
         <v>1</v>
@@ -7706,7 +7703,7 @@
     </row>
     <row r="612" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A612" s="1" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B612">
         <v>1</v>
@@ -7714,7 +7711,7 @@
     </row>
     <row r="613" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A613" s="1" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B613">
         <v>1</v>
@@ -7722,7 +7719,7 @@
     </row>
     <row r="614" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A614" s="1" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B614">
         <v>1</v>
@@ -7730,7 +7727,7 @@
     </row>
     <row r="615" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A615" s="1" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B615">
         <v>1</v>
@@ -7738,7 +7735,7 @@
     </row>
     <row r="616" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A616" s="1" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B616">
         <v>1</v>
@@ -7746,7 +7743,7 @@
     </row>
     <row r="617" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A617" s="1" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B617">
         <v>1</v>
@@ -7754,7 +7751,7 @@
     </row>
     <row r="618" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A618" s="1" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B618">
         <v>1</v>
@@ -7762,7 +7759,7 @@
     </row>
     <row r="619" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A619" s="1" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B619">
         <v>1</v>
@@ -7770,7 +7767,7 @@
     </row>
     <row r="620" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A620" s="1" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B620">
         <v>1</v>
@@ -7778,7 +7775,7 @@
     </row>
     <row r="621" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A621" s="1" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="B621">
         <v>1</v>
@@ -7786,7 +7783,7 @@
     </row>
     <row r="622" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A622" s="1" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B622">
         <v>1</v>
@@ -7794,7 +7791,7 @@
     </row>
     <row r="623" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A623" s="1" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B623">
         <v>1</v>
@@ -7802,7 +7799,7 @@
     </row>
     <row r="624" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A624" s="1" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B624">
         <v>1</v>
@@ -7810,7 +7807,7 @@
     </row>
     <row r="625" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A625" s="1" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B625">
         <v>1</v>
@@ -7818,7 +7815,7 @@
     </row>
     <row r="626" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A626" s="1" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B626">
         <v>1</v>
@@ -7826,7 +7823,7 @@
     </row>
     <row r="627" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A627" s="1" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B627">
         <v>1</v>
@@ -7834,7 +7831,7 @@
     </row>
     <row r="628" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A628" s="1" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="B628">
         <v>1</v>
@@ -7842,7 +7839,7 @@
     </row>
     <row r="629" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A629" s="1" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B629">
         <v>1</v>
@@ -7850,7 +7847,7 @@
     </row>
     <row r="630" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A630" s="1" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B630">
         <v>1</v>
@@ -7858,7 +7855,7 @@
     </row>
     <row r="631" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A631" s="1" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B631">
         <v>1</v>
@@ -7866,7 +7863,7 @@
     </row>
     <row r="632" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A632" s="1" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B632">
         <v>1</v>
@@ -7874,7 +7871,7 @@
     </row>
     <row r="633" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A633" s="1" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B633">
         <v>1</v>
@@ -7882,7 +7879,7 @@
     </row>
     <row r="634" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A634" s="1" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B634">
         <v>1</v>
@@ -7890,15 +7887,15 @@
     </row>
     <row r="635" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A635" s="1" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B635">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="636" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A636" s="1" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B636">
         <v>0</v>
@@ -7906,7 +7903,7 @@
     </row>
     <row r="637" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A637" s="1" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B637">
         <v>0</v>
@@ -7914,7 +7911,7 @@
     </row>
     <row r="638" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A638" s="1" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B638">
         <v>0</v>
@@ -7922,7 +7919,7 @@
     </row>
     <row r="639" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A639" s="1" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="B639">
         <v>0</v>
@@ -7930,7 +7927,7 @@
     </row>
     <row r="640" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A640" s="1" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="B640">
         <v>0</v>
@@ -7938,7 +7935,7 @@
     </row>
     <row r="641" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A641" s="1" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B641">
         <v>0</v>
@@ -7946,7 +7943,7 @@
     </row>
     <row r="642" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A642" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="B642">
         <v>0</v>
@@ -7954,15 +7951,15 @@
     </row>
     <row r="643" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A643" s="1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B643">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="644" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A644" s="1" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B644">
         <v>1</v>
@@ -7970,7 +7967,7 @@
     </row>
     <row r="645" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A645" s="1" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="B645">
         <v>1</v>
@@ -7978,7 +7975,7 @@
     </row>
     <row r="646" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A646" s="1" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B646">
         <v>1</v>
@@ -7986,15 +7983,15 @@
     </row>
     <row r="647" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A647" s="1" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B647">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="648" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A648" s="1" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B648">
         <v>0</v>
@@ -8002,7 +7999,7 @@
     </row>
     <row r="649" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A649" s="1" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="B649">
         <v>0</v>
@@ -8010,23 +8007,23 @@
     </row>
     <row r="650" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A650" s="1" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B650">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="651" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A651" s="1" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="B651">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="652" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A652" s="1" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="B652">
         <v>0</v>
@@ -8034,7 +8031,7 @@
     </row>
     <row r="653" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A653" s="1" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="B653">
         <v>0</v>
@@ -8042,7 +8039,7 @@
     </row>
     <row r="654" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A654" s="1" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="B654">
         <v>0</v>
@@ -8050,7 +8047,7 @@
     </row>
     <row r="655" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A655" s="1" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B655">
         <v>0</v>
@@ -8058,7 +8055,7 @@
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A656" s="1" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B656">
         <v>0</v>
@@ -8066,7 +8063,7 @@
     </row>
     <row r="657" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A657" s="1" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="B657">
         <v>0</v>
@@ -8074,7 +8071,7 @@
     </row>
     <row r="658" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A658" s="1" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="B658">
         <v>0</v>
@@ -8082,7 +8079,7 @@
     </row>
     <row r="659" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A659" s="1" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="B659">
         <v>0</v>
@@ -8090,7 +8087,7 @@
     </row>
     <row r="660" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A660" s="1" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B660">
         <v>0</v>
@@ -8098,15 +8095,15 @@
     </row>
     <row r="661" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A661" s="1" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B661">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="662" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A662" s="1" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="B662">
         <v>1</v>
@@ -8114,7 +8111,7 @@
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A663" s="1" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B663">
         <v>1</v>
@@ -8122,7 +8119,7 @@
     </row>
     <row r="664" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A664" s="1" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B664">
         <v>1</v>
@@ -8130,15 +8127,15 @@
     </row>
     <row r="665" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A665" s="1" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B665">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="666" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A666" s="1" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B666">
         <v>0</v>
@@ -8146,7 +8143,7 @@
     </row>
     <row r="667" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A667" s="1" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B667">
         <v>0</v>
@@ -8154,23 +8151,23 @@
     </row>
     <row r="668" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A668" s="1" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="B668">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="669" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A669" s="1" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="B669">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A670" s="1" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="B670">
         <v>0</v>
@@ -8178,7 +8175,7 @@
     </row>
     <row r="671" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A671" s="1" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="B671">
         <v>0</v>
@@ -8186,7 +8183,7 @@
     </row>
     <row r="672" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A672" s="1" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="B672">
         <v>0</v>
@@ -8194,15 +8191,15 @@
     </row>
     <row r="673" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A673" s="1" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B673">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="674" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A674" s="1" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B674">
         <v>1</v>
@@ -8210,7 +8207,7 @@
     </row>
     <row r="675" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A675" s="1" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B675">
         <v>1</v>
@@ -8218,7 +8215,7 @@
     </row>
     <row r="676" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A676" s="1" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="B676">
         <v>1</v>
@@ -8226,7 +8223,7 @@
     </row>
     <row r="677" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A677" s="1" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="B677">
         <v>1</v>
@@ -8234,7 +8231,7 @@
     </row>
     <row r="678" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A678" s="1" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="B678">
         <v>1</v>
@@ -8242,7 +8239,7 @@
     </row>
     <row r="679" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A679" s="1" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="B679">
         <v>1</v>
@@ -8250,7 +8247,7 @@
     </row>
     <row r="680" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A680" s="1" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B680">
         <v>1</v>
@@ -8258,7 +8255,7 @@
     </row>
     <row r="681" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A681" s="1" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B681">
         <v>1</v>
@@ -8266,7 +8263,7 @@
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A682" s="1" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B682">
         <v>1</v>
@@ -8274,7 +8271,7 @@
     </row>
     <row r="683" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A683" s="1" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B683">
         <v>1</v>
@@ -8282,7 +8279,7 @@
     </row>
     <row r="684" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A684" s="1" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B684">
         <v>1</v>
@@ -8290,7 +8287,7 @@
     </row>
     <row r="685" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A685" s="1" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="B685">
         <v>1</v>
@@ -8298,7 +8295,7 @@
     </row>
     <row r="686" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A686" s="1" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B686">
         <v>1</v>
@@ -8306,7 +8303,7 @@
     </row>
     <row r="687" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A687" s="1" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="B687">
         <v>1</v>
@@ -8314,7 +8311,7 @@
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A688" s="1" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B688">
         <v>1</v>
@@ -8322,7 +8319,7 @@
     </row>
     <row r="689" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A689" s="1" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="B689">
         <v>1</v>
@@ -8330,7 +8327,7 @@
     </row>
     <row r="690" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A690" s="1" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="B690">
         <v>1</v>
@@ -8338,7 +8335,7 @@
     </row>
     <row r="691" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A691" s="1" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="B691">
         <v>1</v>
@@ -8346,7 +8343,7 @@
     </row>
     <row r="692" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A692" s="1" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B692">
         <v>1</v>
@@ -8354,7 +8351,7 @@
     </row>
     <row r="693" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A693" s="1" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="B693">
         <v>1</v>
@@ -8362,7 +8359,7 @@
     </row>
     <row r="694" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A694" s="1" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="B694">
         <v>1</v>
@@ -8370,7 +8367,7 @@
     </row>
     <row r="695" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A695" s="1" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="B695">
         <v>1</v>
@@ -8378,7 +8375,7 @@
     </row>
     <row r="696" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A696" s="1" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="B696">
         <v>1</v>
@@ -8386,7 +8383,7 @@
     </row>
     <row r="697" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A697" s="1" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="B697">
         <v>1</v>
@@ -8394,7 +8391,7 @@
     </row>
     <row r="698" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A698" s="1" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B698">
         <v>1</v>
@@ -8402,7 +8399,7 @@
     </row>
     <row r="699" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A699" s="1" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="B699">
         <v>1</v>
@@ -8410,15 +8407,15 @@
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A700" s="1" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="B700">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A701" s="1" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="B701">
         <v>0</v>
@@ -8426,7 +8423,7 @@
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A702" s="1" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B702">
         <v>0</v>
@@ -8434,15 +8431,15 @@
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A703" s="1" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="B703">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A704" s="1" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B704">
         <v>1</v>
@@ -8450,7 +8447,7 @@
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A705" s="1" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B705">
         <v>1</v>
@@ -8458,7 +8455,7 @@
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A706" s="1" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B706">
         <v>1</v>
@@ -8466,7 +8463,7 @@
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A707" s="1" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="B707">
         <v>1</v>
@@ -8474,7 +8471,7 @@
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A708" s="1" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B708">
         <v>1</v>
@@ -8482,7 +8479,7 @@
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A709" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B709">
         <v>1</v>
@@ -8490,7 +8487,7 @@
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A710" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B710">
         <v>1</v>
@@ -8498,7 +8495,7 @@
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A711" s="1" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B711">
         <v>1</v>
@@ -8506,7 +8503,7 @@
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A712" s="1" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B712">
         <v>1</v>
@@ -8514,7 +8511,7 @@
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A713" s="1" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B713">
         <v>1</v>
@@ -8522,7 +8519,7 @@
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A714" s="1" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B714">
         <v>1</v>
@@ -8530,7 +8527,7 @@
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A715" s="1" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B715">
         <v>1</v>
@@ -8538,7 +8535,7 @@
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A716" s="1" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B716">
         <v>1</v>
@@ -8546,7 +8543,7 @@
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A717" s="1" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="B717">
         <v>1</v>
@@ -8554,7 +8551,7 @@
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A718" s="1" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B718">
         <v>1</v>
@@ -8562,15 +8559,15 @@
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A719" s="1" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B719">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A720" s="1" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B720">
         <v>0</v>
@@ -8578,7 +8575,7 @@
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A721" s="1" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="B721">
         <v>0</v>
@@ -8586,15 +8583,15 @@
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A722" s="1" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="B722">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A723" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B723">
         <v>1</v>
@@ -8602,23 +8599,23 @@
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A724" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B724">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A725" s="1" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B725">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A726" s="1" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B726">
         <v>1</v>
@@ -8626,7 +8623,7 @@
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A727" s="1" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B727">
         <v>1</v>
@@ -8634,7 +8631,7 @@
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A728" s="1" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B728">
         <v>1</v>
@@ -8642,7 +8639,7 @@
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A729" s="1" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B729">
         <v>1</v>
@@ -8650,7 +8647,7 @@
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A730" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B730">
         <v>1</v>
@@ -8658,7 +8655,7 @@
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A731" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B731">
         <v>1</v>
@@ -8666,7 +8663,7 @@
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A732" s="1" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="B732">
         <v>1</v>
@@ -8674,7 +8671,7 @@
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A733" s="1" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B733">
         <v>1</v>
@@ -8682,7 +8679,7 @@
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A734" s="1" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B734">
         <v>1</v>
@@ -8690,7 +8687,7 @@
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A735" s="1" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="B735">
         <v>1</v>
@@ -8698,7 +8695,7 @@
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A736" s="1" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B736">
         <v>1</v>
@@ -8706,7 +8703,7 @@
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A737" s="1" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="B737">
         <v>1</v>
@@ -8714,7 +8711,7 @@
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A738" s="1" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="B738">
         <v>1</v>
@@ -8722,7 +8719,7 @@
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A739" s="1" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B739">
         <v>1</v>
@@ -8730,7 +8727,7 @@
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A740" s="1" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="B740">
         <v>1</v>
@@ -8738,15 +8735,15 @@
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A741" s="1" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B741">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A742" s="1" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="B742">
         <v>0</v>
@@ -8754,7 +8751,7 @@
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A743" s="1" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="B743">
         <v>0</v>
@@ -8762,7 +8759,7 @@
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A744" s="1" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="B744">
         <v>0</v>
@@ -8770,7 +8767,7 @@
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A745" s="1" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B745">
         <v>0</v>
@@ -8778,17 +8775,9 @@
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A746" s="1" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="B746">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="747" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A747" s="1" t="s">
-        <v>743</v>
-      </c>
-      <c r="B747">
         <v>0</v>
       </c>
     </row>

</xml_diff>